<commit_message>
Creando ej. 5 y 6
</commit_message>
<xml_diff>
--- a/Libro1.xlsx
+++ b/Libro1.xlsx
@@ -5,40 +5,32 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PSeInt\Semana 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PSeInt\Semana 4\Pruebas-Escritorio\Pruebas-Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69C24A4-13EA-437F-BC21-A999CC676232}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2811BD-D94D-4663-9257-B696668B3812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{87F55F13-9DAD-43A7-ABF4-42348A9FC45D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{87F55F13-9DAD-43A7-ABF4-42348A9FC45D}"/>
   </bookViews>
   <sheets>
     <sheet name="Ej.1" sheetId="1" r:id="rId1"/>
     <sheet name="Ej.2" sheetId="2" r:id="rId2"/>
     <sheet name="ej.3" sheetId="3" r:id="rId3"/>
     <sheet name="ej.4" sheetId="4" r:id="rId4"/>
+    <sheet name="ej.5" sheetId="5" r:id="rId5"/>
+    <sheet name="ej.6" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="158">
   <si>
     <t>Proceso/SubProcesoLinea(inst)</t>
   </si>
@@ -347,6 +339,171 @@
   </si>
   <si>
     <t>1:GRANEL42(1)</t>
+  </si>
+  <si>
+    <t>dias</t>
+  </si>
+  <si>
+    <t>Horas</t>
+  </si>
+  <si>
+    <t>mes</t>
+  </si>
+  <si>
+    <t>Minlectura</t>
+  </si>
+  <si>
+    <t>Minutos</t>
+  </si>
+  <si>
+    <t>Minxmes</t>
+  </si>
+  <si>
+    <t>Minxsemana</t>
+  </si>
+  <si>
+    <t>1:LECTURA8(1)</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (DIAS).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (HORAS).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (MES).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (MINLECTURA).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (MINUTOS).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (MINXMES).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (MINXSEMANA).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>1:LECTURA9(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA11(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA12(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA13(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA14(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA15(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA17(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA18(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA19(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA20(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA21(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA24(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA25(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA26(1)</t>
+  </si>
+  <si>
+    <t>1:LECTURA28(1)</t>
+  </si>
+  <si>
+    <t>agua6dia</t>
+  </si>
+  <si>
+    <t>Diaspara100mg</t>
+  </si>
+  <si>
+    <t>Dosisdia</t>
+  </si>
+  <si>
+    <t>Dosisretenida</t>
+  </si>
+  <si>
+    <t>lts_agua</t>
+  </si>
+  <si>
+    <t>Mgramosxdia</t>
+  </si>
+  <si>
+    <t>1:VITAMINA9(1)</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (AGUA6DIA).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (DIASPARA100MG).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (DOSISDIA).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (DOSISRETENIDA).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (LTS_AGUA).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;Variable no inicializada (MGRAMOSXDIA).&gt;&gt;</t>
+  </si>
+  <si>
+    <t>1:VITAMINA10(1)</t>
+  </si>
+  <si>
+    <t>1:VITAMINA12(1)</t>
+  </si>
+  <si>
+    <t>1:VITAMINA13(1)</t>
+  </si>
+  <si>
+    <t>1:VITAMINA14(1)</t>
+  </si>
+  <si>
+    <t>1:VITAMINA15(1)</t>
+  </si>
+  <si>
+    <t>1:VITAMINA16(1)</t>
+  </si>
+  <si>
+    <t>1:VITAMINA18(1)</t>
+  </si>
+  <si>
+    <t>1:VITAMINA19(1)</t>
+  </si>
+  <si>
+    <t>1:VITAMINA20(1)</t>
+  </si>
+  <si>
+    <t>1:VITAMINA22(1)</t>
+  </si>
+  <si>
+    <t>1:VITAMINA23(1)</t>
+  </si>
+  <si>
+    <t>1:VITAMINA24(1)</t>
   </si>
 </sst>
 </file>
@@ -394,9 +551,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1467,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECB8A70A-5DA2-4DAA-9A86-6981750AA2C7}">
   <dimension ref="A3:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="37" zoomScaleNormal="37" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L20"/>
+    <sheetView zoomScale="37" zoomScaleNormal="37" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2363,4 +2521,818 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5347FA2-B5BC-4908-8D60-C395D8AB4394}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection sqref="A1:I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="34.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" customWidth="1"/>
+    <col min="6" max="6" width="40.42578125" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" customWidth="1"/>
+    <col min="8" max="8" width="37.5703125" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" t="s">
+        <v>116</v>
+      </c>
+      <c r="H2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" t="s">
+        <v>116</v>
+      </c>
+      <c r="H3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" t="s">
+        <v>113</v>
+      </c>
+      <c r="E4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" t="s">
+        <v>116</v>
+      </c>
+      <c r="H7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>113</v>
+      </c>
+      <c r="E8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>125</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>113</v>
+      </c>
+      <c r="E10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F10" s="2">
+        <v>26666666667</v>
+      </c>
+      <c r="G10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="2">
+        <v>613333333333</v>
+      </c>
+      <c r="F11" s="2">
+        <v>26666666667</v>
+      </c>
+      <c r="G11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="2">
+        <v>613333333333</v>
+      </c>
+      <c r="F12" s="2">
+        <v>26666666667</v>
+      </c>
+      <c r="G12" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" s="2">
+        <v>3066666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>8</v>
+      </c>
+      <c r="D13" s="2">
+        <v>533333333333</v>
+      </c>
+      <c r="E13" s="2">
+        <v>613333333333</v>
+      </c>
+      <c r="F13" s="2">
+        <v>26666666667</v>
+      </c>
+      <c r="G13" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" s="2">
+        <v>3066666666667</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14" s="2">
+        <v>533333333333</v>
+      </c>
+      <c r="E14" s="2">
+        <v>613333333333</v>
+      </c>
+      <c r="F14" s="2">
+        <v>26666666667</v>
+      </c>
+      <c r="G14" s="2">
+        <v>12266666666667</v>
+      </c>
+      <c r="H14" s="2">
+        <v>3066666666667</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="D15" s="2">
+        <v>533333333333</v>
+      </c>
+      <c r="E15" s="2">
+        <v>613333333333</v>
+      </c>
+      <c r="F15" s="2">
+        <v>26666666667</v>
+      </c>
+      <c r="G15" s="2">
+        <v>12266666666667</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3066666666667</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>8</v>
+      </c>
+      <c r="D16" s="2">
+        <v>533333333333</v>
+      </c>
+      <c r="E16" s="2">
+        <v>613333333333</v>
+      </c>
+      <c r="F16" s="2">
+        <v>26666666667</v>
+      </c>
+      <c r="G16" s="2">
+        <v>12266666666667</v>
+      </c>
+      <c r="H16" s="2">
+        <v>3066666666667</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17" s="2">
+        <v>533333333333</v>
+      </c>
+      <c r="E17" s="2">
+        <v>613333333333</v>
+      </c>
+      <c r="F17" s="2">
+        <v>26666666667</v>
+      </c>
+      <c r="G17" s="2">
+        <v>12266666666667</v>
+      </c>
+      <c r="H17" s="2">
+        <v>3066666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA73888-4295-450F-AEC7-BE5A47B43479}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" customWidth="1"/>
+    <col min="5" max="5" width="41.5703125" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" customWidth="1"/>
+    <col min="7" max="7" width="41.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" t="s">
+        <v>136</v>
+      </c>
+      <c r="F1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" t="s">
+        <v>144</v>
+      </c>
+      <c r="G5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D7">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>143</v>
+      </c>
+      <c r="F7" t="s">
+        <v>144</v>
+      </c>
+      <c r="G7" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8">
+        <v>75</v>
+      </c>
+      <c r="E8" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C9" t="s">
+        <v>141</v>
+      </c>
+      <c r="D9">
+        <v>75</v>
+      </c>
+      <c r="E9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B10">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D10">
+        <v>75</v>
+      </c>
+      <c r="E10" t="s">
+        <v>143</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11">
+        <v>75</v>
+      </c>
+      <c r="E11" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2">
+        <v>66666666667</v>
+      </c>
+      <c r="D12">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2">
+        <v>66666666667</v>
+      </c>
+      <c r="D13">
+        <v>75</v>
+      </c>
+      <c r="E13" t="s">
+        <v>143</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2">
+        <v>66666666667</v>
+      </c>
+      <c r="D14">
+        <v>75</v>
+      </c>
+      <c r="E14" t="s">
+        <v>143</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>